<commit_message>
Updated to use CLI for deploying model
</commit_message>
<xml_diff>
--- a/Create Variables for MLOpsPy.xlsx
+++ b/Create Variables for MLOpsPy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>ACI_DEPLOYMENT_NAME</t>
   </si>
@@ -37,9 +37,6 @@
     <t>BASE_NAME</t>
   </si>
   <si>
-    <t>LKHMLOpsPy</t>
-  </si>
-  <si>
     <t>LOCATION</t>
   </si>
   <si>
@@ -86,6 +83,15 @@
   </si>
   <si>
     <t>mlopspy-aks</t>
+  </si>
+  <si>
+    <t>To create a variable group in Azure DevOps, click Pipelines &gt; Library &gt; + Variable group</t>
+  </si>
+  <si>
+    <t>Add the following variables into devopsforai-aml-vg</t>
+  </si>
+  <si>
+    <t>&lt;specify a unique name&gt;</t>
   </si>
 </sst>
 </file>
@@ -426,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -436,102 +442,112 @@
     <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.4">
-      <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="23.4">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="23.4">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23.4">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
         <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>